<commit_message>
Estoy trabajando en la creacion de registros de pz-lp
</commit_message>
<xml_diff>
--- a/Listado PAN y PP 181219.xlsx
+++ b/Listado PAN y PP 181219.xlsx
@@ -920,6 +920,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -928,9 +931,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1216,7 +1216,7 @@
   <dimension ref="A1:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1225,7 @@
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1235,52 +1235,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>60</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>61</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>67</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>70</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>74</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>85</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>86</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>89</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>95</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>97</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>100</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>101</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>105</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>109</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>221</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>117</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>118</v>
       </c>
@@ -4018,7 +4018,7 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="23" t="s">
+      <c r="A103" s="20" t="s">
         <v>167</v>
       </c>
       <c r="B103" s="4">
@@ -4076,7 +4076,7 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="23" t="s">
+      <c r="A105" s="20" t="s">
         <v>170</v>
       </c>
       <c r="B105" s="4">
@@ -4105,7 +4105,7 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="23" t="s">
+      <c r="A106" s="20" t="s">
         <v>173</v>
       </c>
       <c r="B106" s="4">
@@ -4130,7 +4130,7 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="23" t="s">
+      <c r="A107" s="20" t="s">
         <v>174</v>
       </c>
       <c r="B107" s="4">
@@ -4155,7 +4155,7 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="23" t="s">
+      <c r="A108" s="20" t="s">
         <v>175</v>
       </c>
       <c r="B108" s="4">
@@ -4760,11 +4760,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K130">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="PP"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="5" showButton="0"/>
     <filterColumn colId="7">
       <filters>

</xml_diff>